<commit_message>
Got to algo 5 with a little cleanup.
</commit_message>
<xml_diff>
--- a/Documents/Algorithms.xlsx
+++ b/Documents/Algorithms.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithm 1" sheetId="1" r:id="rId1"/>
     <sheet name="Algorithm 2" sheetId="2" r:id="rId2"/>
     <sheet name="Algorithm 3" sheetId="3" r:id="rId3"/>
     <sheet name="Algorithm 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Algorithm 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
   <si>
     <t xml:space="preserve">Declare @CountOfScholarships </t>
   </si>
@@ -102,6 +103,27 @@
   </si>
   <si>
     <t>Get Top Ranked Applicant Who Has Not Already Won</t>
+  </si>
+  <si>
+    <t>Declare @CurrentSplitAmount</t>
+  </si>
+  <si>
+    <t>declare @CountOfApplicants</t>
+  </si>
+  <si>
+    <t>Get Scholarship And Applicant Data</t>
+  </si>
+  <si>
+    <t>Set @CurrentAmount and @CountOfApplicants</t>
+  </si>
+  <si>
+    <t>set @Currentsplitamount as @CurrentAmount/@CountOfApplicants</t>
+  </si>
+  <si>
+    <t>Foreach Applicants</t>
+  </si>
+  <si>
+    <t>Set Result with @currentsplitamount</t>
   </si>
 </sst>
 </file>
@@ -784,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -903,4 +925,129 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Got some information in most of the sections.
</commit_message>
<xml_diff>
--- a/Documents/Algorithms.xlsx
+++ b/Documents/Algorithms.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\ScholarshipAwardingProcess\scholarshipawardingprocess\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Documents\scholarshipawardingprocess\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Algorithm 1" sheetId="1" r:id="rId1"/>
@@ -838,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1088,7 +1088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>